<commit_message>
Update reports and projections
</commit_message>
<xml_diff>
--- a/izvještaji/generated/BHANSA_Januar_2026.xlsx
+++ b/izvještaji/generated/BHANSA_Januar_2026.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N105"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,12 +560,12 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>01/01/2026</t>
+          <t>06/01/2026</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="N3" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -616,12 +616,12 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>01/01/2026</t>
+          <t>06/01/2026</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="N4" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -672,12 +672,12 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>01/01/2026</t>
+          <t>06/01/2026</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="N5" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -728,12 +728,12 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>01/01/2026</t>
+          <t>06/01/2026</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J6" s="4" t="inlineStr"/>
@@ -774,7 +774,7 @@
       </c>
       <c r="N6" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -784,12 +784,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>02/01/2026</t>
+          <t>07/01/2026</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="N7" s="3" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Wednesday</t>
         </is>
       </c>
     </row>
@@ -840,12 +840,12 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>02/01/2026</t>
+          <t>07/01/2026</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="N8" s="3" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Wednesday</t>
         </is>
       </c>
     </row>
@@ -896,12 +896,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>02/01/2026</t>
+          <t>07/01/2026</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J9" s="4" t="inlineStr"/>
@@ -942,7 +942,7 @@
       </c>
       <c r="N9" s="3" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Wednesday</t>
         </is>
       </c>
     </row>
@@ -952,12 +952,12 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>03/01/2026</t>
+          <t>07/01/2026</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J10" s="4" t="inlineStr"/>
@@ -998,7 +998,7 @@
       </c>
       <c r="N10" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Wednesday</t>
         </is>
       </c>
     </row>
@@ -1008,12 +1008,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>03/01/2026</t>
+          <t>08/01/2026</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J11" s="4" t="inlineStr"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="N11" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -1064,12 +1064,12 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>03/01/2026</t>
+          <t>08/01/2026</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="I12" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J12" s="4" t="inlineStr"/>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="N12" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -1120,12 +1120,12 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>03/01/2026</t>
+          <t>08/01/2026</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>Pegasus Airlines</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="I13" s="3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J13" s="4" t="inlineStr"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="N13" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -1176,12 +1176,12 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>03/01/2026</t>
+          <t>08/01/2026</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J14" s="4" t="inlineStr"/>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="N14" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -1232,12 +1232,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>04/01/2026</t>
+          <t>09/01/2026</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>CGN</t>
         </is>
       </c>
       <c r="J15" s="4" t="inlineStr"/>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="N15" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
     </row>
@@ -1288,12 +1288,12 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>04/01/2026</t>
+          <t>09/01/2026</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="N16" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
     </row>
@@ -1344,12 +1344,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>04/01/2026</t>
+          <t>09/01/2026</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J17" s="4" t="inlineStr"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="N17" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
     </row>
@@ -1400,12 +1400,12 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>04/01/2026</t>
+          <t>10/01/2026</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J18" s="4" t="inlineStr"/>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="N18" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -1456,12 +1456,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>10/01/2026</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>CGN</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J19" s="4" t="inlineStr"/>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="N19" s="3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -1512,12 +1512,12 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>10/01/2026</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J20" s="4" t="inlineStr"/>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="N20" s="3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -1568,12 +1568,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>10/01/2026</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>AJet (Turkish Airlines)</t>
+          <t>Pegasus Airlines</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="N21" s="3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -1624,12 +1624,12 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>10/01/2026</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr"/>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="N22" s="3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -1680,12 +1680,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>06/01/2026</t>
+          <t>11/01/2026</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="N23" s="3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -1736,12 +1736,12 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>06/01/2026</t>
+          <t>11/01/2026</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -1782,7 +1782,7 @@
       </c>
       <c r="N24" s="3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -1792,12 +1792,12 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>06/01/2026</t>
+          <t>11/01/2026</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="N25" s="3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -1848,22 +1848,22 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>06/01/2026</t>
+          <t>11/01/2026</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR MALTA LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>A321</t>
+          <t>UNKNOWN</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>ha-lll</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F26" s="3" t="n">
@@ -1877,13 +1877,13 @@
       </c>
       <c r="I26" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J26" s="4" t="inlineStr"/>
       <c r="K26" s="4" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L26" s="4" t="inlineStr"/>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="N26" s="3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -1904,12 +1904,12 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>07/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="N27" s="3" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -1960,12 +1960,12 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>07/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="N28" s="3" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -2016,12 +2016,12 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>07/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>AJet</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="I29" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>SAW</t>
         </is>
       </c>
       <c r="J29" s="4" t="inlineStr"/>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="N29" s="3" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -2072,12 +2072,12 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>07/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="N30" s="3" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -2128,12 +2128,12 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>08/01/2026</t>
+          <t>13/01/2026</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="N31" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -2184,12 +2184,12 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>08/01/2026</t>
+          <t>13/01/2026</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="I32" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J32" s="4" t="inlineStr"/>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="N32" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -2240,12 +2240,12 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>08/01/2026</t>
+          <t>13/01/2026</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="I33" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J33" s="4" t="inlineStr"/>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="N33" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -2296,12 +2296,12 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>08/01/2026</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
@@ -2325,7 +2325,7 @@
       </c>
       <c r="I34" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J34" s="4" t="inlineStr"/>
@@ -2352,12 +2352,12 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="I35" s="3" t="inlineStr">
         <is>
-          <t>CGN</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J35" s="4" t="inlineStr"/>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="N35" s="3" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -2408,12 +2408,12 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C36" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="I36" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>CGN</t>
         </is>
       </c>
       <c r="J36" s="4" t="inlineStr"/>
@@ -2464,12 +2464,12 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="I37" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J37" s="4" t="inlineStr"/>
@@ -2520,12 +2520,12 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C38" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="I38" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J38" s="4" t="inlineStr"/>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="N38" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
     </row>
@@ -2576,12 +2576,12 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="I39" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J39" s="4" t="inlineStr"/>
@@ -2632,12 +2632,12 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="I40" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J40" s="4" t="inlineStr"/>
@@ -2688,12 +2688,12 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
         <is>
-          <t>Pegasus Airlines</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="I41" s="3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J41" s="4" t="inlineStr"/>
@@ -2744,12 +2744,12 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Pegasus Airlines</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="I42" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>SAW</t>
         </is>
       </c>
       <c r="J42" s="4" t="inlineStr"/>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="I43" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J43" s="4" t="inlineStr"/>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="N43" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -2856,12 +2856,12 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026</t>
+          <t>18/01/2026</t>
         </is>
       </c>
       <c r="C44" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="I44" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J44" s="4" t="inlineStr"/>
@@ -2912,12 +2912,12 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026</t>
+          <t>18/01/2026</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="I45" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J45" s="4" t="inlineStr"/>
@@ -2968,12 +2968,12 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026</t>
+          <t>18/01/2026</t>
         </is>
       </c>
       <c r="C46" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="I46" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J46" s="4" t="inlineStr"/>
@@ -3024,12 +3024,12 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>18/01/2026</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="I47" s="3" t="inlineStr">
         <is>
-          <t>CGN</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J47" s="4" t="inlineStr"/>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="N47" s="3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>19/01/2026</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="I48" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>CGN</t>
         </is>
       </c>
       <c r="J48" s="4" t="inlineStr"/>
@@ -3136,12 +3136,12 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>19/01/2026</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>AJet (Turkish Airlines)</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="I49" s="3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J49" s="4" t="inlineStr"/>
@@ -3192,12 +3192,12 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>19/01/2026</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>AJet</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="I50" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>SAW</t>
         </is>
       </c>
       <c r="J50" s="4" t="inlineStr"/>
@@ -3248,12 +3248,12 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>13/01/2026</t>
+          <t>19/01/2026</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="I51" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J51" s="4" t="inlineStr"/>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="N51" s="3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -3304,12 +3304,12 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>13/01/2026</t>
+          <t>20/01/2026</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="I52" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J52" s="4" t="inlineStr"/>
@@ -3360,12 +3360,12 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>13/01/2026</t>
+          <t>20/01/2026</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="I53" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J53" s="4" t="inlineStr"/>
@@ -3416,12 +3416,12 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>20/01/2026</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
@@ -3445,7 +3445,7 @@
       </c>
       <c r="I54" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J54" s="4" t="inlineStr"/>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="N54" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -3472,12 +3472,12 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>15/01/2026</t>
+          <t>22/01/2026</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="I55" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J55" s="4" t="inlineStr"/>
@@ -3528,12 +3528,12 @@
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>22/01/2026</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
@@ -3557,7 +3557,7 @@
       </c>
       <c r="I56" s="3" t="inlineStr">
         <is>
-          <t>CGN</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J56" s="4" t="inlineStr"/>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="N56" s="3" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -3584,12 +3584,12 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>23/01/2026</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="I57" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>CGN</t>
         </is>
       </c>
       <c r="J57" s="4" t="inlineStr"/>
@@ -3640,12 +3640,12 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>23/01/2026</t>
         </is>
       </c>
       <c r="C58" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
@@ -3669,7 +3669,7 @@
       </c>
       <c r="I58" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J58" s="4" t="inlineStr"/>
@@ -3696,12 +3696,12 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>23/01/2026</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="I59" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J59" s="4" t="inlineStr"/>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="N59" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
     </row>
@@ -3752,12 +3752,12 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C60" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="I60" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J60" s="4" t="inlineStr"/>
@@ -3808,12 +3808,12 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
@@ -3837,7 +3837,7 @@
       </c>
       <c r="I61" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J61" s="4" t="inlineStr"/>
@@ -3864,12 +3864,12 @@
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C62" s="4" t="inlineStr">
         <is>
-          <t>Pegasus Airlines</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="I62" s="3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J62" s="4" t="inlineStr"/>
@@ -3920,12 +3920,12 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C63" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Pegasus Airlines</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="I63" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>SAW</t>
         </is>
       </c>
       <c r="J63" s="4" t="inlineStr"/>
@@ -3976,12 +3976,12 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>18/01/2026</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C64" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
@@ -4005,7 +4005,7 @@
       </c>
       <c r="I64" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J64" s="4" t="inlineStr"/>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="N64" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
@@ -4032,12 +4032,12 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>18/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C65" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="I65" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J65" s="4" t="inlineStr"/>
@@ -4088,12 +4088,12 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>18/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C66" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="I66" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J66" s="4" t="inlineStr"/>
@@ -4144,12 +4144,12 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>18/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C67" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="I67" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J67" s="4" t="inlineStr"/>
@@ -4200,12 +4200,12 @@
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>19/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C68" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="I68" s="3" t="inlineStr">
         <is>
-          <t>CGN</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J68" s="4" t="inlineStr"/>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="N68" s="3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -4256,12 +4256,12 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>19/01/2026</t>
+          <t>26/01/2026</t>
         </is>
       </c>
       <c r="C69" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
@@ -4285,7 +4285,7 @@
       </c>
       <c r="I69" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>CGN</t>
         </is>
       </c>
       <c r="J69" s="4" t="inlineStr"/>
@@ -4312,12 +4312,12 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>19/01/2026</t>
+          <t>26/01/2026</t>
         </is>
       </c>
       <c r="C70" s="4" t="inlineStr">
         <is>
-          <t>AJet (Turkish Airlines)</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="I70" s="3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J70" s="4" t="inlineStr"/>
@@ -4368,12 +4368,12 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>19/01/2026</t>
+          <t>26/01/2026</t>
         </is>
       </c>
       <c r="C71" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>AJet</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="I71" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>SAW</t>
         </is>
       </c>
       <c r="J71" s="4" t="inlineStr"/>
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>20/01/2026</t>
+          <t>26/01/2026</t>
         </is>
       </c>
       <c r="C72" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
@@ -4453,7 +4453,7 @@
       </c>
       <c r="I72" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J72" s="4" t="inlineStr"/>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="N72" s="3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -4480,12 +4480,12 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>20/01/2026</t>
+          <t>27/01/2026</t>
         </is>
       </c>
       <c r="C73" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="I73" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J73" s="4" t="inlineStr"/>
@@ -4536,12 +4536,12 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>20/01/2026</t>
+          <t>27/01/2026</t>
         </is>
       </c>
       <c r="C74" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="I74" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J74" s="4" t="inlineStr"/>
@@ -4592,12 +4592,12 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>22/01/2026</t>
+          <t>27/01/2026</t>
         </is>
       </c>
       <c r="C75" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="I75" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J75" s="4" t="inlineStr"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="N75" s="3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -4648,12 +4648,12 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>22/01/2026</t>
+          <t>29/01/2026</t>
         </is>
       </c>
       <c r="C76" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
@@ -4677,7 +4677,7 @@
       </c>
       <c r="I76" s="3" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J76" s="4" t="inlineStr"/>
@@ -4704,12 +4704,12 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>23/01/2026</t>
+          <t>29/01/2026</t>
         </is>
       </c>
       <c r="C77" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="I77" s="3" t="inlineStr">
         <is>
-          <t>CGN</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="J77" s="4" t="inlineStr"/>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="N77" s="3" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
     </row>
@@ -4760,12 +4760,12 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>23/01/2026</t>
+          <t>30/01/2026</t>
         </is>
       </c>
       <c r="C78" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="I78" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>CGN</t>
         </is>
       </c>
       <c r="J78" s="4" t="inlineStr"/>
@@ -4816,12 +4816,12 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>23/01/2026</t>
+          <t>30/01/2026</t>
         </is>
       </c>
       <c r="C79" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="I79" s="3" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J79" s="4" t="inlineStr"/>
@@ -4872,12 +4872,12 @@
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>30/01/2026</t>
         </is>
       </c>
       <c r="C80" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
@@ -4901,7 +4901,7 @@
       </c>
       <c r="I80" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MST</t>
         </is>
       </c>
       <c r="J80" s="4" t="inlineStr"/>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="N80" s="3" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
     </row>
@@ -4928,12 +4928,12 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C81" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
@@ -4957,7 +4957,7 @@
       </c>
       <c r="I81" s="3" t="inlineStr">
         <is>
-          <t>FMM</t>
+          <t>DTM</t>
         </is>
       </c>
       <c r="J81" s="4" t="inlineStr"/>
@@ -4984,12 +4984,12 @@
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C82" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="I82" s="3" t="inlineStr">
         <is>
-          <t>MLH</t>
+          <t>FMM</t>
         </is>
       </c>
       <c r="J82" s="4" t="inlineStr"/>
@@ -5040,12 +5040,12 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C83" s="4" t="inlineStr">
         <is>
-          <t>Pegasus Airlines</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
@@ -5069,7 +5069,7 @@
       </c>
       <c r="I83" s="3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>MLH</t>
         </is>
       </c>
       <c r="J83" s="4" t="inlineStr"/>
@@ -5096,12 +5096,12 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C84" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Pegasus Airlines</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
@@ -5125,7 +5125,7 @@
       </c>
       <c r="I84" s="3" t="inlineStr">
         <is>
-          <t>MMX</t>
+          <t>SAW</t>
         </is>
       </c>
       <c r="J84" s="4" t="inlineStr"/>
@@ -5152,12 +5152,12 @@
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C85" s="4" t="inlineStr">
         <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
+          <t>Wizz Air Hungary</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="I85" s="3" t="inlineStr">
         <is>
-          <t>DTM</t>
+          <t>MMX</t>
         </is>
       </c>
       <c r="J85" s="4" t="inlineStr"/>
@@ -5197,1126 +5197,6 @@
         </is>
       </c>
       <c r="N85" s="3" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" s="3" t="inlineStr">
-        <is>
-          <t>25/01/2026</t>
-        </is>
-      </c>
-      <c r="C86" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D86" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E86" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F86" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G86" s="3" t="inlineStr"/>
-      <c r="H86" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I86" s="3" t="inlineStr">
-        <is>
-          <t>FMM</t>
-        </is>
-      </c>
-      <c r="J86" s="4" t="inlineStr"/>
-      <c r="K86" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L86" s="4" t="inlineStr"/>
-      <c r="M86" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N86" s="3" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="3" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" s="3" t="inlineStr">
-        <is>
-          <t>25/01/2026</t>
-        </is>
-      </c>
-      <c r="C87" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D87" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E87" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F87" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G87" s="3" t="inlineStr"/>
-      <c r="H87" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I87" s="3" t="inlineStr">
-        <is>
-          <t>MLH</t>
-        </is>
-      </c>
-      <c r="J87" s="4" t="inlineStr"/>
-      <c r="K87" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L87" s="4" t="inlineStr"/>
-      <c r="M87" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N87" s="3" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="3" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" s="3" t="inlineStr">
-        <is>
-          <t>25/01/2026</t>
-        </is>
-      </c>
-      <c r="C88" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E88" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F88" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G88" s="3" t="inlineStr"/>
-      <c r="H88" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I88" s="3" t="inlineStr">
-        <is>
-          <t>HAM</t>
-        </is>
-      </c>
-      <c r="J88" s="4" t="inlineStr"/>
-      <c r="K88" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L88" s="4" t="inlineStr"/>
-      <c r="M88" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N88" s="3" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" s="3" t="inlineStr">
-        <is>
-          <t>26/01/2026</t>
-        </is>
-      </c>
-      <c r="C89" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E89" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F89" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G89" s="3" t="inlineStr"/>
-      <c r="H89" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I89" s="3" t="inlineStr">
-        <is>
-          <t>CGN</t>
-        </is>
-      </c>
-      <c r="J89" s="4" t="inlineStr"/>
-      <c r="K89" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L89" s="4" t="inlineStr"/>
-      <c r="M89" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N89" s="3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="3" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" s="3" t="inlineStr">
-        <is>
-          <t>26/01/2026</t>
-        </is>
-      </c>
-      <c r="C90" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D90" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E90" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F90" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G90" s="3" t="inlineStr"/>
-      <c r="H90" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I90" s="3" t="inlineStr">
-        <is>
-          <t>FMM</t>
-        </is>
-      </c>
-      <c r="J90" s="4" t="inlineStr"/>
-      <c r="K90" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L90" s="4" t="inlineStr"/>
-      <c r="M90" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N90" s="3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>26/01/2026</t>
-        </is>
-      </c>
-      <c r="C91" s="4" t="inlineStr">
-        <is>
-          <t>AJet (Turkish Airlines)</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E91" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F91" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G91" s="3" t="inlineStr"/>
-      <c r="H91" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I91" s="3" t="inlineStr">
-        <is>
-          <t>SAW</t>
-        </is>
-      </c>
-      <c r="J91" s="4" t="inlineStr"/>
-      <c r="K91" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L91" s="4" t="inlineStr"/>
-      <c r="M91" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N91" s="3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" s="3" t="inlineStr">
-        <is>
-          <t>26/01/2026</t>
-        </is>
-      </c>
-      <c r="C92" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E92" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F92" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G92" s="3" t="inlineStr"/>
-      <c r="H92" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I92" s="3" t="inlineStr">
-        <is>
-          <t>MST</t>
-        </is>
-      </c>
-      <c r="J92" s="4" t="inlineStr"/>
-      <c r="K92" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L92" s="4" t="inlineStr"/>
-      <c r="M92" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N92" s="3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" s="3" t="inlineStr">
-        <is>
-          <t>27/01/2026</t>
-        </is>
-      </c>
-      <c r="C93" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E93" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F93" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G93" s="3" t="inlineStr"/>
-      <c r="H93" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I93" s="3" t="inlineStr">
-        <is>
-          <t>DTM</t>
-        </is>
-      </c>
-      <c r="J93" s="4" t="inlineStr"/>
-      <c r="K93" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L93" s="4" t="inlineStr"/>
-      <c r="M93" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N93" s="3" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" s="3" t="inlineStr">
-        <is>
-          <t>27/01/2026</t>
-        </is>
-      </c>
-      <c r="C94" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D94" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E94" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F94" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G94" s="3" t="inlineStr"/>
-      <c r="H94" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I94" s="3" t="inlineStr">
-        <is>
-          <t>MLH</t>
-        </is>
-      </c>
-      <c r="J94" s="4" t="inlineStr"/>
-      <c r="K94" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L94" s="4" t="inlineStr"/>
-      <c r="M94" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N94" s="3" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" s="3" t="inlineStr">
-        <is>
-          <t>27/01/2026</t>
-        </is>
-      </c>
-      <c r="C95" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E95" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F95" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G95" s="3" t="inlineStr"/>
-      <c r="H95" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I95" s="3" t="inlineStr">
-        <is>
-          <t>MMX</t>
-        </is>
-      </c>
-      <c r="J95" s="4" t="inlineStr"/>
-      <c r="K95" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L95" s="4" t="inlineStr"/>
-      <c r="M95" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N95" s="3" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" s="3" t="inlineStr">
-        <is>
-          <t>29/01/2026</t>
-        </is>
-      </c>
-      <c r="C96" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E96" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F96" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G96" s="3" t="inlineStr"/>
-      <c r="H96" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I96" s="3" t="inlineStr">
-        <is>
-          <t>DTM</t>
-        </is>
-      </c>
-      <c r="J96" s="4" t="inlineStr"/>
-      <c r="K96" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L96" s="4" t="inlineStr"/>
-      <c r="M96" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N96" s="3" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" s="3" t="inlineStr">
-        <is>
-          <t>29/01/2026</t>
-        </is>
-      </c>
-      <c r="C97" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D97" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E97" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F97" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G97" s="3" t="inlineStr"/>
-      <c r="H97" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I97" s="3" t="inlineStr">
-        <is>
-          <t>HAM</t>
-        </is>
-      </c>
-      <c r="J97" s="4" t="inlineStr"/>
-      <c r="K97" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L97" s="4" t="inlineStr"/>
-      <c r="M97" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N97" s="3" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="3" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" s="3" t="inlineStr">
-        <is>
-          <t>30/01/2026</t>
-        </is>
-      </c>
-      <c r="C98" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D98" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E98" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F98" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G98" s="3" t="inlineStr"/>
-      <c r="H98" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I98" s="3" t="inlineStr">
-        <is>
-          <t>CGN</t>
-        </is>
-      </c>
-      <c r="J98" s="4" t="inlineStr"/>
-      <c r="K98" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L98" s="4" t="inlineStr"/>
-      <c r="M98" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N98" s="3" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="3" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" s="3" t="inlineStr">
-        <is>
-          <t>30/01/2026</t>
-        </is>
-      </c>
-      <c r="C99" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D99" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E99" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F99" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G99" s="3" t="inlineStr"/>
-      <c r="H99" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I99" s="3" t="inlineStr">
-        <is>
-          <t>FMM</t>
-        </is>
-      </c>
-      <c r="J99" s="4" t="inlineStr"/>
-      <c r="K99" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L99" s="4" t="inlineStr"/>
-      <c r="M99" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N99" s="3" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="3" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" s="3" t="inlineStr">
-        <is>
-          <t>30/01/2026</t>
-        </is>
-      </c>
-      <c r="C100" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D100" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E100" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F100" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G100" s="3" t="inlineStr"/>
-      <c r="H100" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I100" s="3" t="inlineStr">
-        <is>
-          <t>MST</t>
-        </is>
-      </c>
-      <c r="J100" s="4" t="inlineStr"/>
-      <c r="K100" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L100" s="4" t="inlineStr"/>
-      <c r="M100" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N100" s="3" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="3" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" s="3" t="inlineStr">
-        <is>
-          <t>31/01/2026</t>
-        </is>
-      </c>
-      <c r="C101" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D101" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E101" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F101" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G101" s="3" t="inlineStr"/>
-      <c r="H101" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I101" s="3" t="inlineStr">
-        <is>
-          <t>DTM</t>
-        </is>
-      </c>
-      <c r="J101" s="4" t="inlineStr"/>
-      <c r="K101" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L101" s="4" t="inlineStr"/>
-      <c r="M101" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N101" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" s="3" t="inlineStr">
-        <is>
-          <t>31/01/2026</t>
-        </is>
-      </c>
-      <c r="C102" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D102" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E102" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F102" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G102" s="3" t="inlineStr"/>
-      <c r="H102" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I102" s="3" t="inlineStr">
-        <is>
-          <t>FMM</t>
-        </is>
-      </c>
-      <c r="J102" s="4" t="inlineStr"/>
-      <c r="K102" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L102" s="4" t="inlineStr"/>
-      <c r="M102" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N102" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" s="3" t="inlineStr">
-        <is>
-          <t>31/01/2026</t>
-        </is>
-      </c>
-      <c r="C103" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D103" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E103" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F103" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G103" s="3" t="inlineStr"/>
-      <c r="H103" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I103" s="3" t="inlineStr">
-        <is>
-          <t>MLH</t>
-        </is>
-      </c>
-      <c r="J103" s="4" t="inlineStr"/>
-      <c r="K103" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L103" s="4" t="inlineStr"/>
-      <c r="M103" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N103" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" s="3" t="inlineStr">
-        <is>
-          <t>31/01/2026</t>
-        </is>
-      </c>
-      <c r="C104" s="4" t="inlineStr">
-        <is>
-          <t>Pegasus Airlines</t>
-        </is>
-      </c>
-      <c r="D104" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E104" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F104" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G104" s="3" t="inlineStr"/>
-      <c r="H104" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I104" s="3" t="inlineStr">
-        <is>
-          <t>SAW</t>
-        </is>
-      </c>
-      <c r="J104" s="4" t="inlineStr"/>
-      <c r="K104" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L104" s="4" t="inlineStr"/>
-      <c r="M104" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N104" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" s="3" t="inlineStr">
-        <is>
-          <t>31/01/2026</t>
-        </is>
-      </c>
-      <c r="C105" s="4" t="inlineStr">
-        <is>
-          <t>WIZZ AIR HUNGARY LTD</t>
-        </is>
-      </c>
-      <c r="D105" s="3" t="inlineStr">
-        <is>
-          <t>UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E105" s="3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F105" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G105" s="3" t="inlineStr"/>
-      <c r="H105" s="3" t="inlineStr">
-        <is>
-          <t>TZL</t>
-        </is>
-      </c>
-      <c r="I105" s="3" t="inlineStr">
-        <is>
-          <t>MMX</t>
-        </is>
-      </c>
-      <c r="J105" s="4" t="inlineStr"/>
-      <c r="K105" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L105" s="4" t="inlineStr"/>
-      <c r="M105" s="3" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N105" s="3" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>

</xml_diff>